<commit_message>
Novo DER e algumas telas
Novo DER e algumas telas
</commit_message>
<xml_diff>
--- a/ANÁLISE/ESPECIFICAÇÃO CASOS DE USO.xlsx
+++ b/ANÁLISE/ESPECIFICAÇÃO CASOS DE USO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>